<commit_message>
Added more entries to testing DOC
</commit_message>
<xml_diff>
--- a/Documentation/Testēšanas dokuimentācija.xlsx
+++ b/Documentation/Testēšanas dokuimentācija.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karlis.melveris\Personal files\CyberShock\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mazzy\Unity\CyberShock\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A904C98A-E6C7-44BB-90E3-AA9A2186E8CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4446F930-543F-4323-8216-F303A97DB4BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Apraksts" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="257">
   <si>
     <t>Identifikatoru atšifrējums:</t>
   </si>
@@ -430,13 +430,7 @@
     <t>Izvēles dziesmas datu izskata ģenerācija</t>
   </si>
   <si>
-    <t>Ja ir izvēlēta dziesma, tās top 5 augstākie punki ir redzami.</t>
-  </si>
-  <si>
     <t>Ja ir izvēlēta dziesma tās "High score" ir jābūt redzamiem</t>
-  </si>
-  <si>
-    <t>Kreisajā pusē ir redzami 5 augstāk iegūtie punkti dilstoši uz leju.</t>
   </si>
   <si>
     <t>Izvēlnē atpakaļ poga</t>
@@ -470,9 +464,6 @@
     <t>nospiežot izvēnes lapas labajā pusē dziesmu ir jābūt redzamai tie dati kreisajā pusē</t>
   </si>
   <si>
-    <t>Kreisajā pusē var redzēt dziesmas foto, nosaukumu un grūtības iestatījumi.</t>
-  </si>
-  <si>
     <t>TP.IZV.FA.03</t>
   </si>
   <si>
@@ -480,9 +471,6 @@
   </si>
   <si>
     <t>Izvēlnē grūtības iestaījumu pogas satur datus kuri ir saistīti ar grūtības līmeņiem, kurus var izvēlēt un vēlāk lietot citām funkcijām</t>
-  </si>
-  <si>
-    <t>Izvēlētās dziesmas grūtības līmeņi ir redzami un satur datus, kā piemēram nosaukumu un krāsu.</t>
   </si>
   <si>
     <t>1) Izvēlnē tiek izvēlēta dziesma
@@ -544,6 +532,316 @@
   </si>
   <si>
     <t>Atverās dziesmas līmenis</t>
+  </si>
+  <si>
+    <t>TP.IEST.FA.01</t>
+  </si>
+  <si>
+    <t>Mainīt ekrēna rezolūciju</t>
+  </si>
+  <si>
+    <t>TP.IEST.VA.01</t>
+  </si>
+  <si>
+    <t>Maina rezolūcijas iestatījumus</t>
+  </si>
+  <si>
+    <t>1) Atver iestatījumu lapu
+2) Nospiež pa labi vai kreisi
+3) Vērtība palielinās, vai samazinās</t>
+  </si>
+  <si>
+    <t>Kreisais peles klikšķis</t>
+  </si>
+  <si>
+    <t>Skaitli var mainīt, bet nekas cits nemainas</t>
+  </si>
+  <si>
+    <t>TP.IEST.VA.02</t>
+  </si>
+  <si>
+    <t>TP.IEST.VA.03</t>
+  </si>
+  <si>
+    <t>TP.IEST.VA.04</t>
+  </si>
+  <si>
+    <t>Mainīt ekrēna tipu</t>
+  </si>
+  <si>
+    <t>Maina ekrāna tipu iestatījumu</t>
+  </si>
+  <si>
+    <t>1) Atver iestatījumu lapu
+2) Nospiež pa labi vai kreisi
+3) Vērtība mainās</t>
+  </si>
+  <si>
+    <t>Vērtību var mainīt, bet nekas cits nemainas</t>
+  </si>
+  <si>
+    <t>Mainīt spēles kvalitāti</t>
+  </si>
+  <si>
+    <t>Maina spēles kvalitātes iestatījumu</t>
+  </si>
+  <si>
+    <t>Vērtība var mainīt, bet nekas cits nemainas</t>
+  </si>
+  <si>
+    <t>Mainīt spēles skaļumu</t>
+  </si>
+  <si>
+    <t>1) Atver iestatījumu lapu
+2) Mainot slīdni pa labi vai kreisi mainīs skaļumu</t>
+  </si>
+  <si>
+    <t>TP.IEST.VA.05</t>
+  </si>
+  <si>
+    <t>TP.IEST.VA.06</t>
+  </si>
+  <si>
+    <t>PR.IEST.07</t>
+  </si>
+  <si>
+    <t>Iestatīt  izmainītās vērtības</t>
+  </si>
+  <si>
+    <t>1) Atver iestatījumu lapu
+2) Mainot slīdni pa labi vai kreisi mainīs effektu skaļumu</t>
+  </si>
+  <si>
+    <t>1) Atver iestatījumu lapu
+2) Mainot slīdni pa labi vai kreisi mainīs mūzikas skaļumu</t>
+  </si>
+  <si>
+    <t>Kreisais peles klikšķis un turēšana</t>
+  </si>
+  <si>
+    <t>Akseptēt iestatījumus</t>
+  </si>
+  <si>
+    <t>Visi iestaījumi kuri bija tikai mainīti tikai vizuāli, pēc "Apply" nospiešanas tiek saglabāti un iestatīti kā ir noteikts iepriekšējos iestatījuma testa piemēros</t>
+  </si>
+  <si>
+    <t>1) Atver iestatījumus
+2) Nomaina jebkuru iestatijumu kas nav skaļums.
+3) Nospiest "Apply"</t>
+  </si>
+  <si>
+    <t>Kreisais peles klikšķi</t>
+  </si>
+  <si>
+    <t>Iepriekš noteiktās vērtības tiek iestatītas</t>
+  </si>
+  <si>
+    <t>Mainot slīdņa vērtību mainīs visas spēles skaļumu</t>
+  </si>
+  <si>
+    <t>Pēc nospiešanas visas iepriekš noteiktās vērtības tiek saglabātas un lietotas</t>
+  </si>
+  <si>
+    <t>Maina mūzikas skaļumu</t>
+  </si>
+  <si>
+    <t>Maina effektu skaļumu</t>
+  </si>
+  <si>
+    <t>Maina spēles kopējo skaļumu</t>
+  </si>
+  <si>
+    <t>Kreisajā pusē var redzēt dziesmas foto, nosaukumu un grūtības iestatījumi</t>
+  </si>
+  <si>
+    <t>Kreisajā pusē ir redzami 5 augstāk iegūtie punkti dilstoši uz leju</t>
+  </si>
+  <si>
+    <t>Spiežot pa labi vai kreisi izmainīs skaitli kas reprezentē rezolūciju un saglabā šo skaitli xml failā. Mainot šo skaitli nemainīs ekrāna rezolūciju</t>
+  </si>
+  <si>
+    <t>Spiežot pa labi vai kreisi izmainīs nosaukumi kas reprezentē ekrāna tipu (windowed, borderless window, fullscreen) un saglabā šo vērtību xml failā</t>
+  </si>
+  <si>
+    <t>Spiežot pa labi vai kreisi izmainīs spēles kvalitāti no viss vienkāršākā, līdz viss sarežģītākajam un saglabā šo vērtību xml failā</t>
+  </si>
+  <si>
+    <t>Slīdnī var palielināt vai samazināt kopējo spēles skaļumu, no 0% līdz 100%. Šis iestatījums mainās uzreiz pēc izmaiņas</t>
+  </si>
+  <si>
+    <t>Slīdnī var palielināt vai samazināt effektu skaļumu, no 0% līdz 100%. Šis iestatījums mainās uzreiz pēc izmaiņas</t>
+  </si>
+  <si>
+    <t>Slīdnī var palielināt vai samazināt mūzikas skaļumu, no 0% līdz 100%. Šis iestatījums mainās uzreiz pēc izmaiņas</t>
+  </si>
+  <si>
+    <t>Ja ir izvēlēta dziesma, tās top 5 augstākie punki ir redzami</t>
+  </si>
+  <si>
+    <t>Izvēlētās dziesmas grūtības līmeņi ir redzami un satur datus, kā piemēram nosaukumu un krāsu</t>
+  </si>
+  <si>
+    <t>PR.SP.01</t>
+  </si>
+  <si>
+    <t>Jebkurā momentā var pauzēt spēli, lai mainītu iestatījumus vai iziet no līmeņa</t>
+  </si>
+  <si>
+    <t>PR.SP.02</t>
+  </si>
+  <si>
+    <t>PR.SP.03</t>
+  </si>
+  <si>
+    <t>PR.SP.04</t>
+  </si>
+  <si>
+    <t>PR.SP.05</t>
+  </si>
+  <si>
+    <t>PR.SP.06</t>
+  </si>
+  <si>
+    <t>PR.SP.07</t>
+  </si>
+  <si>
+    <t>PR.SP.08</t>
+  </si>
+  <si>
+    <t>PR.SP.09</t>
+  </si>
+  <si>
+    <t>PR.SP.10</t>
+  </si>
+  <si>
+    <t>Izlasa dziesmas datus</t>
+  </si>
+  <si>
+    <t>Lādēšanās ekrāns kurš parādās ja līmeņa ielādēšana aizņem pārāk ilgu laiku</t>
+  </si>
+  <si>
+    <t>Viena spiediena, kreisās pozīcijas poga</t>
+  </si>
+  <si>
+    <t>Viena spiediena, labās pozīcijas poga</t>
+  </si>
+  <si>
+    <t>Viena spiediena, aukšējās pozīcijas poga</t>
+  </si>
+  <si>
+    <t>Viena spiediena, "space" poga</t>
+  </si>
+  <si>
+    <t>Turēšanas, kreisās pozīcijas poga</t>
+  </si>
+  <si>
+    <t>PR.SP.11</t>
+  </si>
+  <si>
+    <t>PR.SP.12</t>
+  </si>
+  <si>
+    <t>PR.SP.13</t>
+  </si>
+  <si>
+    <t>PR.SP.14</t>
+  </si>
+  <si>
+    <t>Turēšanas, labās pozīcijas poga</t>
+  </si>
+  <si>
+    <t>Turēšanas, aukšējās pozīcijas poga</t>
+  </si>
+  <si>
+    <t>Turēšanas, "space" poga</t>
+  </si>
+  <si>
+    <t>Punkti tiek iedoti pēc prasībām</t>
+  </si>
+  <si>
+    <t>Veselību var samazināt</t>
+  </si>
+  <si>
+    <t>Veselību var palielināt</t>
+  </si>
+  <si>
+    <t>PR.SP.15</t>
+  </si>
+  <si>
+    <t>PR.SP.16</t>
+  </si>
+  <si>
+    <t>PR.SP.17</t>
+  </si>
+  <si>
+    <t>PR.SP.18</t>
+  </si>
+  <si>
+    <t>Līmeņa datus var izlasīt</t>
+  </si>
+  <si>
+    <t>Var ielādēt viena spiediena noti/būltu</t>
+  </si>
+  <si>
+    <t>Var ielādēt turēšanas noti/būltu</t>
+  </si>
+  <si>
+    <t>var notiekt notes ātrumu</t>
+  </si>
+  <si>
+    <t>TP.SP.FA.01</t>
+  </si>
+  <si>
+    <t>Iespēja pauzēt spēli</t>
+  </si>
+  <si>
+    <t>Jebkurā momentā nospeiest "esc", lai pauzētu spēli un atvērt jaunu skatu</t>
+  </si>
+  <si>
+    <t>1) Atvērt spēles sadaļu
+2) nospiest "esc"</t>
+  </si>
+  <si>
+    <t>"esc" poga</t>
+  </si>
+  <si>
+    <t>TP.SP.FA.02</t>
+  </si>
+  <si>
+    <t>TP.SP.FA.03</t>
+  </si>
+  <si>
+    <t>Izlasa dziesmu kas ir Map-data folderī</t>
+  </si>
+  <si>
+    <t>Ielādējot jaunu līmeni tiek atskaņota dziesma</t>
+  </si>
+  <si>
+    <t>Atvērta spēles sadaļa ar dziesmas failu</t>
+  </si>
+  <si>
+    <t>Atver pauzēšanas ekrānu</t>
+  </si>
+  <si>
+    <t>Mūzika tiek atskaņota</t>
+  </si>
+  <si>
+    <t>Pievienojot vairākus milzīgus failus "map-data" folderī</t>
+  </si>
+  <si>
+    <t>Lādēšanās ekrāns</t>
+  </si>
+  <si>
+    <t>TP.SP.VA.01</t>
+  </si>
+  <si>
+    <t>Ja faili aizņem pārāk ilgu laiku lai ielādētos ir jābūt redzamam ka spēle lādējas</t>
+  </si>
+  <si>
+    <t>Spēle rāda lādēšanās ekrānu</t>
+  </si>
+  <si>
+    <t>Lādēšanās ekrāns parādas</t>
   </si>
 </sst>
 </file>
@@ -730,7 +1028,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -775,6 +1073,12 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -811,11 +1115,8 @@
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1161,28 +1462,28 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -1205,80 +1506,80 @@
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="22"/>
+      <c r="C9" s="24"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="22"/>
+      <c r="C10" s="24"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="22"/>
+      <c r="C11" s="24"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="22"/>
+      <c r="C12" s="24"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="22"/>
+      <c r="C13" s="24"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="22"/>
+      <c r="C14" s="24"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="22"/>
+      <c r="C15" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1300,11 +1601,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1322,8 +1623,8 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -1342,10 +1643,10 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="29"/>
+      <c r="B5" s="31"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
@@ -1372,10 +1673,10 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="29"/>
+      <c r="B9" s="31"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
@@ -1434,10 +1735,10 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="29"/>
+      <c r="B17" s="31"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
@@ -1488,30 +1789,167 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="28" t="s">
+      <c r="A24" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="29"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="19"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="19"/>
+      <c r="B25" s="31"/>
+    </row>
+    <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="36" t="s">
+        <v>203</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="19"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="19"/>
+      <c r="A27" s="36" t="s">
+        <v>205</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="36" t="s">
+        <v>206</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="19"/>
+      <c r="A29" s="36" t="s">
+        <v>207</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="36" t="s">
+        <v>208</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="36" t="s">
+        <v>209</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="36" t="s">
+        <v>210</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="36" t="s">
+        <v>211</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="36" t="s">
+        <v>212</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="36" t="s">
+        <v>213</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="36" t="s">
+        <v>221</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="36" t="s">
+        <v>222</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="36" t="s">
+        <v>224</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="36" t="s">
+        <v>231</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="36" t="s">
+        <v>232</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="36" t="s">
+        <v>233</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="36" t="s">
+        <v>234</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>238</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="A25:B25"/>
     <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A24:B24"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A9:B9"/>
@@ -1523,11 +1961,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1569,16 +2007,16 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
     </row>
     <row r="3" spans="1:8" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
@@ -1633,14 +2071,14 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
     </row>
     <row r="6" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
@@ -1675,10 +2113,10 @@
       <c r="B7" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="C7" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="D7" s="34" t="s">
+      <c r="C7" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="D7" s="22" t="s">
         <v>102</v>
       </c>
       <c r="E7" s="21" t="s">
@@ -1687,7 +2125,7 @@
       <c r="F7" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="G7" s="34" t="s">
+      <c r="G7" s="22" t="s">
         <v>105</v>
       </c>
       <c r="H7" s="21" t="s">
@@ -1695,16 +2133,16 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="C8" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="D8" s="34" t="s">
+      <c r="C8" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="D8" s="22" t="s">
         <v>111</v>
       </c>
       <c r="E8" s="16" t="s">
@@ -1713,7 +2151,7 @@
       <c r="F8" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="G8" s="34" t="s">
+      <c r="G8" s="22" t="s">
         <v>112</v>
       </c>
       <c r="H8" s="16" t="s">
@@ -1721,35 +2159,35 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
+      <c r="A9" s="34"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
     </row>
     <row r="10" spans="1:8" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="D10" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="E10" s="34" t="s">
+      <c r="E10" s="22" t="s">
         <v>116</v>
       </c>
       <c r="F10" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="G10" s="34" t="s">
+      <c r="G10" s="22" t="s">
         <v>121</v>
       </c>
       <c r="H10" s="16" t="s">
@@ -1757,156 +2195,156 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="D11" s="34" t="s">
-        <v>138</v>
-      </c>
-      <c r="E11" s="34" t="s">
+      <c r="D11" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="E11" s="22" t="s">
         <v>122</v>
       </c>
       <c r="F11" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="G11" s="34" t="s">
-        <v>139</v>
+      <c r="G11" s="22" t="s">
+        <v>193</v>
       </c>
       <c r="H11" s="16" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="D12" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="D12" s="34" t="s">
-        <v>127</v>
-      </c>
-      <c r="E12" s="34" t="s">
+      <c r="E12" s="22" t="s">
         <v>122</v>
       </c>
       <c r="F12" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="G12" s="34" t="s">
-        <v>128</v>
+      <c r="G12" s="22" t="s">
+        <v>194</v>
       </c>
       <c r="H12" s="16" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="D13" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="B13" s="34" t="s">
-        <v>129</v>
-      </c>
-      <c r="C13" s="34" t="s">
+      <c r="E13" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="D13" s="34" t="s">
+      <c r="F13" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="G13" s="22" t="s">
         <v>135</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="G13" s="34" t="s">
-        <v>137</v>
       </c>
       <c r="H13" s="20" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A14" s="34" t="s">
+      <c r="A14" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="E14" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="B14" s="34" t="s">
+      <c r="F14" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="G14" s="22" t="s">
         <v>141</v>
-      </c>
-      <c r="C14" s="34" t="s">
-        <v>142</v>
-      </c>
-      <c r="D14" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="E14" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="G14" s="34" t="s">
-        <v>145</v>
       </c>
       <c r="H14" s="20" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
-        <v>146</v>
-      </c>
-      <c r="B15" s="34" t="s">
+      <c r="A15" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="E15" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="F15" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="D15" s="34" t="s">
+      <c r="G15" s="22" t="s">
         <v>149</v>
-      </c>
-      <c r="E15" s="34" t="s">
-        <v>151</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="G15" s="34" t="s">
-        <v>153</v>
       </c>
       <c r="H15" s="20" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="120" x14ac:dyDescent="0.25">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="E16" s="22" t="s">
         <v>154</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="F16" s="22" t="s">
         <v>155</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="G16" s="22" t="s">
         <v>156</v>
-      </c>
-      <c r="D16" s="34" t="s">
-        <v>157</v>
-      </c>
-      <c r="E16" s="34" t="s">
-        <v>158</v>
-      </c>
-      <c r="F16" s="34" t="s">
-        <v>159</v>
-      </c>
-      <c r="G16" s="34" t="s">
-        <v>160</v>
       </c>
       <c r="H16" s="20" t="s">
         <v>73</v>
@@ -1922,21 +2360,381 @@
       <c r="G17" s="34"/>
       <c r="H17" s="34"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="34"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
+    <row r="18" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="G18" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="G19" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="H19" s="20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="G20" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="H20" s="20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>192</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G21" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="H21" s="20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>191</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G22" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="H22" s="20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="D23" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="F23" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G23" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="H23" s="20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A24" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="F24" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="G24" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="H24" s="20" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="34"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+    </row>
+    <row r="26" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="22" t="s">
+        <v>239</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>242</v>
+      </c>
+      <c r="F26" s="22" t="s">
+        <v>243</v>
+      </c>
+      <c r="G26" s="22" t="s">
+        <v>249</v>
+      </c>
+      <c r="H26" s="20" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="22" t="s">
+        <v>244</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="C27" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="D27" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="E27" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="F27" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="G27" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="H27" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="D28" s="22" t="s">
+        <v>255</v>
+      </c>
+      <c r="E28" s="22" t="s">
+        <v>251</v>
+      </c>
+      <c r="F28" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="G28" s="22" t="s">
+        <v>256</v>
+      </c>
+      <c r="H28" s="20" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="22" t="s">
+        <v>245</v>
+      </c>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="20" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="22"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="20" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="22"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="20" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="22"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="20"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="22"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="20"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="22"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="20"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="22"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="20"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="22"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="20"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="22"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A5:H5"/>
     <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A25:H25"/>
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1991,16 +2789,16 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
     </row>
     <row r="3" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -2095,14 +2893,14 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
     </row>
     <row r="3" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">

</xml_diff>

<commit_message>
added pause and UI fixes
</commit_message>
<xml_diff>
--- a/Documentation/Testēšanas dokuimentācija.xlsx
+++ b/Documentation/Testēšanas dokuimentācija.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karlis.melveris\Personal files\CyberShock\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mazzy\Unity\CyberShock\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A58AB706-C208-460A-A69B-A2C670B97B44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013A7B98-3D43-4EEA-A915-FC25ECE4FD87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6690" yWindow="3465" windowWidth="38565" windowHeight="15435" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Apraksts" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="289">
   <si>
     <t>Identifikatoru atšifrējums:</t>
   </si>
@@ -723,9 +723,6 @@
     <t>PR.SP.11</t>
   </si>
   <si>
-    <t>PR.SP.12</t>
-  </si>
-  <si>
     <t>Punkti tiek iedoti pēc prasībām</t>
   </si>
   <si>
@@ -948,6 +945,9 @@
   </si>
   <si>
     <t>Punkti un reitngs vienmēr ir vienādi sarp visiem gadījumiem kur ir redzami</t>
+  </si>
+  <si>
+    <t>TP.SP.FA.09</t>
   </si>
 </sst>
 </file>
@@ -1707,7 +1707,7 @@
   <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
@@ -1934,7 +1934,7 @@
         <v>207</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -1942,7 +1942,7 @@
         <v>208</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1950,7 +1950,7 @@
         <v>209</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1958,7 +1958,7 @@
         <v>210</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1966,7 +1966,7 @@
         <v>211</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1974,7 +1974,7 @@
         <v>212</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1982,7 +1982,7 @@
         <v>213</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1990,13 +1990,11 @@
         <v>216</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="20" t="s">
-        <v>217</v>
-      </c>
+      <c r="A37" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2013,11 +2011,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G36" sqref="G36"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2606,25 +2604,25 @@
     </row>
     <row r="26" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="B26" s="22" t="s">
         <v>223</v>
       </c>
-      <c r="B26" s="22" t="s">
+      <c r="C26" s="22" t="s">
         <v>224</v>
-      </c>
-      <c r="C26" s="22" t="s">
-        <v>225</v>
       </c>
       <c r="D26" s="22" t="s">
         <v>204</v>
       </c>
       <c r="E26" s="22" t="s">
+        <v>225</v>
+      </c>
+      <c r="F26" s="22" t="s">
         <v>226</v>
       </c>
-      <c r="F26" s="22" t="s">
-        <v>227</v>
-      </c>
       <c r="G26" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H26" s="20" t="s">
         <v>203</v>
@@ -2632,25 +2630,25 @@
     </row>
     <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B27" s="19" t="s">
         <v>214</v>
       </c>
       <c r="C27" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="D27" s="22" t="s">
         <v>229</v>
       </c>
-      <c r="D27" s="22" t="s">
+      <c r="E27" s="22" t="s">
         <v>230</v>
-      </c>
-      <c r="E27" s="22" t="s">
-        <v>231</v>
       </c>
       <c r="F27" s="22" t="s">
         <v>186</v>
       </c>
       <c r="G27" s="22" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H27" s="20" t="s">
         <v>205</v>
@@ -2658,25 +2656,25 @@
     </row>
     <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
+        <v>235</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="C28" s="22" t="s">
         <v>236</v>
       </c>
-      <c r="B28" s="22" t="s">
-        <v>235</v>
-      </c>
-      <c r="C28" s="22" t="s">
+      <c r="D28" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="D28" s="22" t="s">
-        <v>238</v>
-      </c>
       <c r="E28" s="22" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F28" s="22" t="s">
         <v>186</v>
       </c>
       <c r="G28" s="22" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H28" s="20" t="s">
         <v>206</v>
@@ -2684,25 +2682,25 @@
     </row>
     <row r="29" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C29" s="22" t="s">
+        <v>244</v>
+      </c>
+      <c r="D29" s="22" t="s">
+        <v>243</v>
+      </c>
+      <c r="E29" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="F29" s="22" t="s">
         <v>245</v>
       </c>
-      <c r="D29" s="22" t="s">
-        <v>244</v>
-      </c>
-      <c r="E29" s="22" t="s">
-        <v>248</v>
-      </c>
-      <c r="F29" s="22" t="s">
-        <v>246</v>
-      </c>
       <c r="G29" s="22" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H29" s="21" t="s">
         <v>207</v>
@@ -2710,25 +2708,25 @@
     </row>
     <row r="30" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C30" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="D30" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="E30" s="22" t="s">
         <v>247</v>
       </c>
-      <c r="D30" s="22" t="s">
-        <v>253</v>
-      </c>
-      <c r="E30" s="22" t="s">
-        <v>248</v>
-      </c>
       <c r="F30" s="22" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G30" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H30" s="21" t="s">
         <v>207</v>
@@ -2736,25 +2734,25 @@
     </row>
     <row r="31" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B31" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="C31" s="22" t="s">
         <v>251</v>
       </c>
-      <c r="C31" s="22" t="s">
-        <v>252</v>
-      </c>
       <c r="D31" s="22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F31" s="22" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G31" s="22" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H31" s="21" t="s">
         <v>207</v>
@@ -2762,25 +2760,25 @@
     </row>
     <row r="32" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B32" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="C32" s="22" t="s">
         <v>258</v>
       </c>
-      <c r="C32" s="22" t="s">
+      <c r="D32" s="22" t="s">
         <v>259</v>
       </c>
-      <c r="D32" s="22" t="s">
+      <c r="E32" s="22" t="s">
         <v>260</v>
       </c>
-      <c r="E32" s="22" t="s">
-        <v>261</v>
-      </c>
       <c r="F32" s="22" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G32" s="22" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H32" s="21" t="s">
         <v>208</v>
@@ -2788,25 +2786,25 @@
     </row>
     <row r="33" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="22" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B33" s="22" t="s">
+        <v>267</v>
+      </c>
+      <c r="C33" s="22" t="s">
+        <v>258</v>
+      </c>
+      <c r="D33" s="22" t="s">
         <v>268</v>
       </c>
-      <c r="C33" s="22" t="s">
-        <v>259</v>
-      </c>
-      <c r="D33" s="22" t="s">
+      <c r="E33" s="22" t="s">
+        <v>270</v>
+      </c>
+      <c r="F33" s="22" t="s">
+        <v>245</v>
+      </c>
+      <c r="G33" s="22" t="s">
         <v>269</v>
-      </c>
-      <c r="E33" s="22" t="s">
-        <v>271</v>
-      </c>
-      <c r="F33" s="22" t="s">
-        <v>246</v>
-      </c>
-      <c r="G33" s="22" t="s">
-        <v>270</v>
       </c>
       <c r="H33" s="21" t="s">
         <v>208</v>
@@ -2814,25 +2812,25 @@
     </row>
     <row r="34" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B34" s="22" t="s">
+        <v>271</v>
+      </c>
+      <c r="C34" s="22" t="s">
         <v>272</v>
       </c>
-      <c r="C34" s="22" t="s">
+      <c r="D34" s="22" t="s">
         <v>273</v>
       </c>
-      <c r="D34" s="22" t="s">
+      <c r="E34" s="22" t="s">
+        <v>276</v>
+      </c>
+      <c r="F34" s="22" t="s">
+        <v>275</v>
+      </c>
+      <c r="G34" s="22" t="s">
         <v>274</v>
-      </c>
-      <c r="E34" s="22" t="s">
-        <v>277</v>
-      </c>
-      <c r="F34" s="22" t="s">
-        <v>276</v>
-      </c>
-      <c r="G34" s="22" t="s">
-        <v>275</v>
       </c>
       <c r="H34" s="21" t="s">
         <v>209</v>
@@ -2840,25 +2838,25 @@
     </row>
     <row r="35" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B35" s="22" t="s">
+        <v>277</v>
+      </c>
+      <c r="C35" s="22" t="s">
         <v>278</v>
       </c>
-      <c r="C35" s="22" t="s">
+      <c r="D35" s="22" t="s">
+        <v>280</v>
+      </c>
+      <c r="E35" s="22" t="s">
         <v>279</v>
       </c>
-      <c r="D35" s="22" t="s">
+      <c r="F35" s="22" t="s">
+        <v>245</v>
+      </c>
+      <c r="G35" s="22" t="s">
         <v>281</v>
-      </c>
-      <c r="E35" s="22" t="s">
-        <v>280</v>
-      </c>
-      <c r="F35" s="22" t="s">
-        <v>246</v>
-      </c>
-      <c r="G35" s="22" t="s">
-        <v>282</v>
       </c>
       <c r="H35" s="21" t="s">
         <v>210</v>
@@ -2866,39 +2864,48 @@
     </row>
     <row r="36" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="s">
+        <v>284</v>
+      </c>
+      <c r="B36" s="22" t="s">
+        <v>282</v>
+      </c>
+      <c r="C36" s="22" t="s">
         <v>285</v>
       </c>
-      <c r="B36" s="22" t="s">
-        <v>283</v>
-      </c>
-      <c r="C36" s="22" t="s">
+      <c r="D36" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="D36" s="22" t="s">
+      <c r="E36" s="22" t="s">
+        <v>279</v>
+      </c>
+      <c r="F36" s="22" t="s">
+        <v>245</v>
+      </c>
+      <c r="G36" s="22" t="s">
         <v>287</v>
-      </c>
-      <c r="E36" s="22" t="s">
-        <v>280</v>
-      </c>
-      <c r="F36" s="22" t="s">
-        <v>246</v>
-      </c>
-      <c r="G36" s="22" t="s">
-        <v>288</v>
       </c>
       <c r="H36" s="21" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="22"/>
+      <c r="A37" s="22" t="s">
+        <v>288</v>
+      </c>
       <c r="B37" s="22"/>
       <c r="C37" s="22"/>
       <c r="D37" s="22"/>
       <c r="E37" s="22"/>
       <c r="F37" s="22"/>
       <c r="G37" s="22"/>
-      <c r="H37" s="20"/>
+      <c r="H37" s="21" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H38" s="21" t="s">
+        <v>213</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>